<commit_message>
add Rmd summarizing catches
</commit_message>
<xml_diff>
--- a/data/southcoastCUs.xlsx
+++ b/data/southcoastCUs.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="319" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="364" uniqueCount="116">
   <si>
     <t>Region</t>
   </si>
@@ -273,6 +273,105 @@
   </si>
   <si>
     <t>Presence of US strays likely driving current estimates</t>
+  </si>
+  <si>
+    <t>WSP BMs, short-term trend and prob. of decline suggest poor status</t>
+  </si>
+  <si>
+    <t>Evidence suggests it may be red/amber, but data is of poor quality (redd counts, infrequently surveyed)</t>
+  </si>
+  <si>
+    <t>Data only available for 1 of 7 sites</t>
+  </si>
+  <si>
+    <t>WSP BMs, extent of decline and abs. abundance suggest green, but short term-decline resulted in provisional status</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Declining trends and low abundance suggest red, but only single site surveyed and may not be representative </t>
+  </si>
+  <si>
+    <t>Rel. abundance and short-term trend suggest red, but high uncertainty</t>
+  </si>
+  <si>
+    <t>Mixed signals from metrics; small decline, not all sites are declining and total abundance is above COSEWIC D</t>
+  </si>
+  <si>
+    <t>Enhanced so not assessed</t>
+  </si>
+  <si>
+    <t>Relative abundance and short-term trend are poor, but decline extent is amber</t>
+  </si>
+  <si>
+    <t>Designated as red due to high exploitation and straying from hatcheries rather than abundance/trends</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rel. abundance, trend and prob. of decline all are poor; very small hatchery contributions </t>
+  </si>
+  <si>
+    <t>Abundance and trend are red, but imprecise visual estimates that could be biased low and anecdotal large recent return</t>
+  </si>
+  <si>
+    <t>No biological BMs and short spawner TS</t>
+  </si>
+  <si>
+    <t>Driven by non-WSP considerations: small portion of total abundance in wild sites and lots of straying</t>
+  </si>
+  <si>
+    <t>Low quality data</t>
+  </si>
+  <si>
+    <t>No recent escapement estimates</t>
+  </si>
+  <si>
+    <t>Low quality data and potentially extirpated</t>
+  </si>
+  <si>
+    <t>Low quality data, but may be abundant</t>
+  </si>
+  <si>
+    <t>Baker, Bridge, Chilako, Chilcotin, Endako, Narcosli, Naver, West Road, Baezaeko, Cottonwood, Horsefly, Nazko</t>
+  </si>
+  <si>
+    <t>Current surveys may underestimate abundance due to large watershed size</t>
+  </si>
+  <si>
+    <t>Adams, Little, South Thompson, Thompson</t>
+  </si>
+  <si>
+    <t>May not be a distinct CU (part of Middle Shuswap)</t>
+  </si>
+  <si>
+    <t>Bessette, Duteau</t>
+  </si>
+  <si>
+    <t>Relatively little basic information for this CU; absolute abundance likely much greater than relative index</t>
+  </si>
+  <si>
+    <t>Blue, Finn</t>
+  </si>
+  <si>
+    <t>Okanagan</t>
+  </si>
+  <si>
+    <t>Barriere, Lemieux, Mahood, Clearwater, Raft</t>
+  </si>
+  <si>
+    <t>Represents succesful recolonization from Lower Shuswap</t>
+  </si>
+  <si>
+    <t>Adams (upper)</t>
+  </si>
+  <si>
+    <t>No havitat based benchmarks and low quality data</t>
+  </si>
+  <si>
+    <t>Big Silver</t>
+  </si>
+  <si>
+    <t>One of the largest and most intensively studied populations; status may be corrupted by hatchery contributions</t>
+  </si>
+  <si>
+    <t>Harrison River</t>
   </si>
 </sst>
 </file>
@@ -614,24 +713,24 @@
   <dimension ref="A1:N37"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <pane xSplit="4" ySplit="1" topLeftCell="H2" activePane="bottomRight" state="frozen"/>
-      <selection pane="topRight" activeCell="E1" sqref="E1"/>
+      <pane xSplit="3" ySplit="1" topLeftCell="L8" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="I7" sqref="I7"/>
+      <selection pane="bottomRight" activeCell="M12" sqref="M12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" width="12.109375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="29" style="4" customWidth="1"/>
-    <col min="4" max="4" width="11.44140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="7.88671875" customWidth="1"/>
-    <col min="6" max="6" width="8.5546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="8.21875" customWidth="1"/>
-    <col min="8" max="8" width="8.44140625" customWidth="1"/>
-    <col min="11" max="11" width="10.88671875" customWidth="1"/>
-    <col min="13" max="13" width="37" style="4" customWidth="1"/>
-    <col min="14" max="14" width="25" customWidth="1"/>
+    <col min="4" max="4" width="7.88671875" customWidth="1"/>
+    <col min="5" max="5" width="8.5546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8.21875" customWidth="1"/>
+    <col min="7" max="7" width="8.44140625" customWidth="1"/>
+    <col min="10" max="10" width="10.88671875" customWidth="1"/>
+    <col min="12" max="12" width="41.77734375" style="4" customWidth="1"/>
+    <col min="13" max="13" width="32" style="4" customWidth="1"/>
+    <col min="14" max="14" width="32.5546875" style="4" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.3">
@@ -645,60 +744,60 @@
         <v>1</v>
       </c>
       <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1"/>
+      <c r="F1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="J1" s="2"/>
+      <c r="K1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="L1" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="M1" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="N1" s="2" t="s">
         <v>2</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="F1" s="1"/>
-      <c r="G1" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="H1" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="I1" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="J1" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="K1" s="2"/>
-      <c r="L1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="M1" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="N1" s="1" t="s">
-        <v>17</v>
       </c>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A2" s="1"/>
       <c r="B2" s="1"/>
       <c r="C2" s="2"/>
-      <c r="D2" s="1"/>
+      <c r="D2" s="3" t="s">
+        <v>18</v>
+      </c>
       <c r="E2" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="F2" s="3" t="s">
         <v>19</v>
       </c>
+      <c r="F2" s="2"/>
       <c r="G2" s="2"/>
       <c r="H2" s="2"/>
-      <c r="I2" s="2"/>
+      <c r="I2" s="5" t="s">
+        <v>28</v>
+      </c>
       <c r="J2" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="K2" s="5" t="s">
         <v>76</v>
       </c>
-      <c r="L2" s="1"/>
+      <c r="K2" s="1"/>
+      <c r="L2" s="2"/>
       <c r="M2" s="2"/>
-      <c r="N2" s="1"/>
-    </row>
-    <row r="3" spans="1:14" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="N2" s="2"/>
+    </row>
+    <row r="3" spans="1:14" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>9</v>
       </c>
@@ -708,35 +807,38 @@
       <c r="C3" s="4" t="s">
         <v>11</v>
       </c>
+      <c r="D3" t="s">
+        <v>12</v>
+      </c>
       <c r="E3" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="F3" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="G3" t="s">
-        <v>14</v>
-      </c>
-      <c r="H3" t="s">
         <v>15</v>
       </c>
+      <c r="H3">
+        <v>5</v>
+      </c>
       <c r="I3">
-        <v>5</v>
+        <v>4915</v>
       </c>
       <c r="J3">
-        <v>4915</v>
-      </c>
-      <c r="K3">
         <v>22097</v>
       </c>
-      <c r="L3" t="s">
+      <c r="K3" t="s">
         <v>24</v>
       </c>
-      <c r="M3" s="4" t="s">
+      <c r="L3" s="4" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="4" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="N3" s="4" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>9</v>
       </c>
@@ -746,29 +848,35 @@
       <c r="C4" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="E4" t="s">
-        <v>12</v>
+      <c r="D4" t="s">
+        <v>12</v>
+      </c>
+      <c r="F4" t="s">
+        <v>23</v>
       </c>
       <c r="G4" t="s">
-        <v>23</v>
-      </c>
-      <c r="H4" t="s">
         <v>22</v>
       </c>
+      <c r="H4">
+        <v>4</v>
+      </c>
       <c r="I4">
-        <v>4</v>
+        <v>23588</v>
       </c>
       <c r="J4">
-        <v>23588</v>
-      </c>
-      <c r="K4">
         <v>88624</v>
       </c>
-      <c r="L4" t="s">
+      <c r="K4" t="s">
         <v>25</v>
       </c>
+      <c r="L4" s="4" t="s">
+        <v>78</v>
+      </c>
       <c r="M4" s="4" t="s">
-        <v>78</v>
+        <v>102</v>
+      </c>
+      <c r="N4" s="4" t="s">
+        <v>103</v>
       </c>
     </row>
     <row r="5" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
@@ -781,35 +889,41 @@
       <c r="C5" s="4" t="s">
         <v>26</v>
       </c>
+      <c r="D5" t="s">
+        <v>12</v>
+      </c>
       <c r="E5" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="F5" t="s">
-        <v>13</v>
+        <v>23</v>
       </c>
       <c r="G5" t="s">
-        <v>23</v>
-      </c>
-      <c r="H5" t="s">
         <v>15</v>
       </c>
+      <c r="H5">
+        <v>4</v>
+      </c>
       <c r="I5">
-        <v>4</v>
+        <v>215</v>
       </c>
       <c r="J5">
-        <v>215</v>
-      </c>
-      <c r="K5">
         <v>853</v>
       </c>
-      <c r="L5" t="s">
+      <c r="K5" t="s">
         <v>24</v>
       </c>
+      <c r="L5" s="4" t="s">
+        <v>79</v>
+      </c>
       <c r="M5" s="4" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="6" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
+        <v>104</v>
+      </c>
+      <c r="N5" s="4" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>9</v>
       </c>
@@ -819,32 +933,38 @@
       <c r="C6" s="4" t="s">
         <v>27</v>
       </c>
+      <c r="D6" t="s">
+        <v>12</v>
+      </c>
       <c r="E6" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="F6" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="G6" t="s">
-        <v>14</v>
-      </c>
-      <c r="H6" t="s">
         <v>15</v>
       </c>
-      <c r="I6">
+      <c r="H6">
         <v>5</v>
       </c>
+      <c r="I6" t="s">
+        <v>46</v>
+      </c>
       <c r="J6" t="s">
         <v>46</v>
       </c>
       <c r="K6" t="s">
-        <v>46</v>
-      </c>
-      <c r="L6" t="s">
         <v>24</v>
       </c>
+      <c r="L6" s="4" t="s">
+        <v>80</v>
+      </c>
       <c r="M6" s="4" t="s">
-        <v>80</v>
+        <v>106</v>
+      </c>
+      <c r="N6" s="4" t="s">
+        <v>107</v>
       </c>
     </row>
     <row r="7" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
@@ -857,38 +977,41 @@
       <c r="C7" s="4" t="s">
         <v>31</v>
       </c>
+      <c r="D7" t="s">
+        <v>12</v>
+      </c>
       <c r="E7" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="F7" t="s">
-        <v>13</v>
+        <v>23</v>
       </c>
       <c r="G7" t="s">
-        <v>23</v>
-      </c>
-      <c r="H7" t="s">
         <v>22</v>
       </c>
+      <c r="H7">
+        <v>4</v>
+      </c>
       <c r="I7">
-        <v>4</v>
+        <v>367</v>
       </c>
       <c r="J7">
-        <v>367</v>
-      </c>
-      <c r="K7">
         <v>2848</v>
       </c>
-      <c r="L7" t="s">
+      <c r="K7" t="s">
         <v>24</v>
       </c>
+      <c r="L7" s="4" t="s">
+        <v>81</v>
+      </c>
       <c r="M7" s="4" t="s">
-        <v>81</v>
-      </c>
-      <c r="N7" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="N7" s="4" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>9</v>
       </c>
@@ -898,32 +1021,38 @@
       <c r="C8" s="4" t="s">
         <v>32</v>
       </c>
+      <c r="D8" t="s">
+        <v>12</v>
+      </c>
       <c r="E8" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="F8" t="s">
-        <v>13</v>
+        <v>23</v>
       </c>
       <c r="G8" t="s">
-        <v>23</v>
-      </c>
-      <c r="H8" t="s">
         <v>15</v>
       </c>
+      <c r="H8">
+        <v>5</v>
+      </c>
       <c r="I8">
-        <v>5</v>
+        <v>1684</v>
       </c>
       <c r="J8">
-        <v>1684</v>
-      </c>
-      <c r="K8">
         <v>7822</v>
       </c>
-      <c r="L8" t="s">
+      <c r="K8" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="L8" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="N8" s="4" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>9</v>
       </c>
@@ -933,32 +1062,41 @@
       <c r="C9" s="4" t="s">
         <v>33</v>
       </c>
+      <c r="D9" t="s">
+        <v>12</v>
+      </c>
       <c r="E9" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="F9" t="s">
-        <v>13</v>
+        <v>23</v>
       </c>
       <c r="G9" t="s">
-        <v>23</v>
-      </c>
-      <c r="H9" t="s">
         <v>22</v>
       </c>
-      <c r="I9">
+      <c r="H9">
         <v>5</v>
       </c>
+      <c r="I9" t="s">
+        <v>46</v>
+      </c>
       <c r="J9" t="s">
         <v>46</v>
       </c>
       <c r="K9" t="s">
-        <v>46</v>
-      </c>
-      <c r="L9" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="L9" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="M9" s="4" t="s">
+        <v>110</v>
+      </c>
+      <c r="N9" s="4" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>9</v>
       </c>
@@ -968,32 +1106,41 @@
       <c r="C10" s="4" t="s">
         <v>34</v>
       </c>
+      <c r="D10" t="s">
+        <v>12</v>
+      </c>
       <c r="E10" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="F10" t="s">
-        <v>13</v>
+        <v>23</v>
       </c>
       <c r="G10" t="s">
-        <v>23</v>
-      </c>
-      <c r="H10" t="s">
         <v>15</v>
       </c>
-      <c r="I10">
+      <c r="H10">
         <v>5</v>
       </c>
+      <c r="I10" t="s">
+        <v>46</v>
+      </c>
       <c r="J10" t="s">
         <v>46</v>
       </c>
       <c r="K10" t="s">
-        <v>46</v>
-      </c>
-      <c r="L10" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="L10" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="M10" s="4" t="s">
+        <v>112</v>
+      </c>
+      <c r="N10" s="4" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>9</v>
       </c>
@@ -1003,32 +1150,41 @@
       <c r="C11" s="4" t="s">
         <v>35</v>
       </c>
+      <c r="D11" t="s">
+        <v>12</v>
+      </c>
       <c r="E11" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="F11" t="s">
-        <v>13</v>
+        <v>44</v>
       </c>
       <c r="G11" t="s">
-        <v>44</v>
-      </c>
-      <c r="H11" t="s">
         <v>22</v>
       </c>
+      <c r="H11">
+        <v>4</v>
+      </c>
       <c r="I11">
-        <v>4</v>
+        <v>15318</v>
       </c>
       <c r="J11">
-        <v>15318</v>
-      </c>
-      <c r="K11">
         <v>63808</v>
       </c>
-      <c r="L11" t="s">
+      <c r="K11" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="12" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="L11" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="M11" s="4" t="s">
+        <v>114</v>
+      </c>
+      <c r="N11" s="4" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>9</v>
       </c>
@@ -1038,29 +1194,32 @@
       <c r="C12" s="4" t="s">
         <v>36</v>
       </c>
+      <c r="D12" t="s">
+        <v>12</v>
+      </c>
       <c r="E12" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="F12" t="s">
-        <v>13</v>
+        <v>23</v>
       </c>
       <c r="G12" t="s">
-        <v>23</v>
-      </c>
-      <c r="H12" t="s">
         <v>15</v>
       </c>
+      <c r="H12">
+        <v>5</v>
+      </c>
       <c r="I12">
-        <v>5</v>
+        <v>246</v>
       </c>
       <c r="J12">
-        <v>246</v>
-      </c>
-      <c r="K12">
         <v>988</v>
       </c>
-      <c r="L12" t="s">
+      <c r="K12" t="s">
         <v>49</v>
+      </c>
+      <c r="L12" s="4" t="s">
+        <v>87</v>
       </c>
     </row>
     <row r="13" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
@@ -1073,32 +1232,35 @@
       <c r="C13" s="4" t="s">
         <v>37</v>
       </c>
+      <c r="D13" t="s">
+        <v>12</v>
+      </c>
       <c r="E13" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="F13" t="s">
-        <v>13</v>
+        <v>44</v>
       </c>
       <c r="G13" t="s">
-        <v>44</v>
-      </c>
-      <c r="H13" t="s">
         <v>15</v>
       </c>
+      <c r="H13">
+        <v>5</v>
+      </c>
       <c r="I13">
-        <v>5</v>
+        <v>329</v>
       </c>
       <c r="J13">
-        <v>329</v>
-      </c>
-      <c r="K13">
         <v>1351</v>
       </c>
-      <c r="L13" t="s">
+      <c r="K13" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="L13" s="4" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>9</v>
       </c>
@@ -1108,29 +1270,32 @@
       <c r="C14" s="4" t="s">
         <v>38</v>
       </c>
+      <c r="D14" t="s">
+        <v>12</v>
+      </c>
       <c r="E14" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="F14" t="s">
-        <v>13</v>
+        <v>23</v>
       </c>
       <c r="G14" t="s">
-        <v>23</v>
-      </c>
-      <c r="H14" t="s">
         <v>15</v>
       </c>
+      <c r="H14">
+        <v>5</v>
+      </c>
       <c r="I14">
-        <v>5</v>
+        <v>5373</v>
       </c>
       <c r="J14">
-        <v>5373</v>
-      </c>
-      <c r="K14">
         <v>25322</v>
       </c>
-      <c r="L14" t="s">
+      <c r="K14" t="s">
         <v>50</v>
+      </c>
+      <c r="L14" s="4" t="s">
+        <v>89</v>
       </c>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.3">
@@ -1143,29 +1308,32 @@
       <c r="C15" s="4" t="s">
         <v>39</v>
       </c>
+      <c r="D15" t="s">
+        <v>45</v>
+      </c>
       <c r="E15" t="s">
-        <v>45</v>
+        <v>12</v>
       </c>
       <c r="F15" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="G15" t="s">
-        <v>14</v>
-      </c>
-      <c r="H15" t="s">
         <v>15</v>
       </c>
+      <c r="H15">
+        <v>5</v>
+      </c>
       <c r="I15">
-        <v>5</v>
+        <v>332</v>
       </c>
       <c r="J15">
-        <v>332</v>
-      </c>
-      <c r="K15">
         <v>1368</v>
       </c>
-      <c r="L15" t="s">
+      <c r="K15" t="s">
         <v>51</v>
+      </c>
+      <c r="L15" s="4" t="s">
+        <v>90</v>
       </c>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.3">
@@ -1178,29 +1346,32 @@
       <c r="C16" s="4" t="s">
         <v>40</v>
       </c>
+      <c r="D16" t="s">
+        <v>45</v>
+      </c>
       <c r="E16" t="s">
-        <v>45</v>
+        <v>12</v>
       </c>
       <c r="F16" t="s">
-        <v>12</v>
+        <v>44</v>
       </c>
       <c r="G16" t="s">
-        <v>44</v>
-      </c>
-      <c r="H16" t="s">
         <v>22</v>
       </c>
-      <c r="I16">
+      <c r="H16">
         <v>3</v>
       </c>
+      <c r="I16" t="s">
+        <v>46</v>
+      </c>
       <c r="J16" t="s">
         <v>46</v>
       </c>
       <c r="K16" t="s">
-        <v>46</v>
-      </c>
-      <c r="L16" t="s">
         <v>51</v>
+      </c>
+      <c r="L16" s="4" t="s">
+        <v>90</v>
       </c>
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.3">
@@ -1213,29 +1384,32 @@
       <c r="C17" s="4" t="s">
         <v>48</v>
       </c>
+      <c r="D17" t="s">
+        <v>45</v>
+      </c>
       <c r="E17" t="s">
-        <v>45</v>
+        <v>12</v>
       </c>
       <c r="F17" t="s">
-        <v>12</v>
+        <v>44</v>
       </c>
       <c r="G17" t="s">
-        <v>44</v>
-      </c>
-      <c r="H17" t="s">
         <v>22</v>
       </c>
+      <c r="H17">
+        <v>4</v>
+      </c>
       <c r="I17">
-        <v>4</v>
+        <v>98</v>
       </c>
       <c r="J17">
-        <v>98</v>
-      </c>
-      <c r="K17">
         <v>960</v>
       </c>
-      <c r="L17" t="s">
+      <c r="K17" t="s">
         <v>51</v>
+      </c>
+      <c r="L17" s="4" t="s">
+        <v>90</v>
       </c>
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.3">
@@ -1248,29 +1422,32 @@
       <c r="C18" s="4" t="s">
         <v>47</v>
       </c>
+      <c r="D18" t="s">
+        <v>46</v>
+      </c>
       <c r="E18" t="s">
-        <v>46</v>
+        <v>12</v>
       </c>
       <c r="F18" t="s">
-        <v>12</v>
+        <v>44</v>
       </c>
       <c r="G18" t="s">
-        <v>44</v>
-      </c>
-      <c r="H18" t="s">
         <v>22</v>
       </c>
+      <c r="H18">
+        <v>3</v>
+      </c>
       <c r="I18">
-        <v>3</v>
+        <v>999</v>
       </c>
       <c r="J18">
-        <v>999</v>
-      </c>
-      <c r="K18">
         <v>5537</v>
       </c>
-      <c r="L18" t="s">
+      <c r="K18" t="s">
         <v>51</v>
+      </c>
+      <c r="L18" s="4" t="s">
+        <v>90</v>
       </c>
     </row>
     <row r="19" spans="1:12" x14ac:dyDescent="0.3">
@@ -1283,29 +1460,32 @@
       <c r="C19" s="4" t="s">
         <v>41</v>
       </c>
+      <c r="D19" t="s">
+        <v>45</v>
+      </c>
       <c r="E19" t="s">
-        <v>45</v>
+        <v>12</v>
       </c>
       <c r="F19" t="s">
-        <v>12</v>
+        <v>44</v>
       </c>
       <c r="G19" t="s">
-        <v>44</v>
-      </c>
-      <c r="H19" t="s">
         <v>22</v>
       </c>
-      <c r="I19">
+      <c r="H19">
         <v>4</v>
       </c>
+      <c r="I19" t="s">
+        <v>46</v>
+      </c>
       <c r="J19" t="s">
         <v>46</v>
       </c>
       <c r="K19" t="s">
-        <v>46</v>
-      </c>
-      <c r="L19" t="s">
         <v>51</v>
+      </c>
+      <c r="L19" s="4" t="s">
+        <v>90</v>
       </c>
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.3">
@@ -1318,29 +1498,32 @@
       <c r="C20" s="4" t="s">
         <v>42</v>
       </c>
+      <c r="D20" t="s">
+        <v>13</v>
+      </c>
       <c r="E20" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F20" t="s">
-        <v>12</v>
+        <v>23</v>
       </c>
       <c r="G20" t="s">
-        <v>23</v>
-      </c>
-      <c r="H20" t="s">
         <v>22</v>
       </c>
+      <c r="H20">
+        <v>4</v>
+      </c>
       <c r="I20">
-        <v>4</v>
+        <v>15</v>
       </c>
       <c r="J20">
-        <v>15</v>
-      </c>
-      <c r="K20">
         <v>200</v>
       </c>
-      <c r="L20" t="s">
+      <c r="K20" t="s">
         <v>51</v>
+      </c>
+      <c r="L20" s="4" t="s">
+        <v>90</v>
       </c>
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.3">
@@ -1353,29 +1536,32 @@
       <c r="C21" s="4" t="s">
         <v>43</v>
       </c>
+      <c r="D21" t="s">
+        <v>45</v>
+      </c>
       <c r="E21" t="s">
-        <v>45</v>
+        <v>12</v>
       </c>
       <c r="F21" t="s">
-        <v>12</v>
+        <v>44</v>
       </c>
       <c r="G21" t="s">
-        <v>44</v>
-      </c>
-      <c r="H21" t="s">
         <v>22</v>
       </c>
+      <c r="H21">
+        <v>3</v>
+      </c>
       <c r="I21">
-        <v>3</v>
+        <v>318</v>
       </c>
       <c r="J21">
-        <v>318</v>
-      </c>
-      <c r="K21">
         <v>2570</v>
       </c>
-      <c r="L21" t="s">
+      <c r="K21" t="s">
         <v>51</v>
+      </c>
+      <c r="L21" s="4" t="s">
+        <v>90</v>
       </c>
     </row>
     <row r="22" spans="1:12" x14ac:dyDescent="0.3">
@@ -1388,29 +1574,32 @@
       <c r="C22" s="4" t="s">
         <v>56</v>
       </c>
+      <c r="D22" t="s">
+        <v>45</v>
+      </c>
       <c r="E22" t="s">
-        <v>45</v>
+        <v>12</v>
       </c>
       <c r="F22" t="s">
-        <v>12</v>
+        <v>23</v>
       </c>
       <c r="G22" t="s">
-        <v>23</v>
-      </c>
-      <c r="H22" t="s">
         <v>22</v>
       </c>
+      <c r="H22">
+        <v>4</v>
+      </c>
       <c r="I22">
-        <v>4</v>
+        <v>2094</v>
       </c>
       <c r="J22">
-        <v>2094</v>
-      </c>
-      <c r="K22">
         <v>13470</v>
       </c>
-      <c r="L22" t="s">
+      <c r="K22" t="s">
         <v>51</v>
+      </c>
+      <c r="L22" s="4" t="s">
+        <v>90</v>
       </c>
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.3">
@@ -1423,29 +1612,32 @@
       <c r="C23" s="4" t="s">
         <v>57</v>
       </c>
+      <c r="D23" t="s">
+        <v>45</v>
+      </c>
       <c r="E23" t="s">
-        <v>45</v>
+        <v>12</v>
       </c>
       <c r="F23" t="s">
-        <v>12</v>
+        <v>23</v>
       </c>
       <c r="G23" t="s">
-        <v>23</v>
-      </c>
-      <c r="H23" t="s">
         <v>22</v>
       </c>
+      <c r="H23">
+        <v>4</v>
+      </c>
       <c r="I23">
-        <v>4</v>
+        <v>249</v>
       </c>
       <c r="J23">
-        <v>249</v>
-      </c>
-      <c r="K23">
         <v>2094</v>
       </c>
-      <c r="L23" t="s">
+      <c r="K23" t="s">
         <v>51</v>
+      </c>
+      <c r="L23" s="4" t="s">
+        <v>90</v>
       </c>
     </row>
     <row r="24" spans="1:12" x14ac:dyDescent="0.3">
@@ -1458,29 +1650,32 @@
       <c r="C24" s="4" t="s">
         <v>58</v>
       </c>
+      <c r="D24" t="s">
+        <v>45</v>
+      </c>
       <c r="E24" t="s">
-        <v>45</v>
+        <v>12</v>
       </c>
       <c r="F24" t="s">
-        <v>12</v>
+        <v>44</v>
       </c>
       <c r="G24" t="s">
-        <v>44</v>
-      </c>
-      <c r="H24" t="s">
         <v>22</v>
       </c>
+      <c r="H24">
+        <v>4</v>
+      </c>
       <c r="I24">
-        <v>4</v>
+        <v>620</v>
       </c>
       <c r="J24">
-        <v>620</v>
-      </c>
-      <c r="K24">
         <v>5500</v>
       </c>
-      <c r="L24" t="s">
+      <c r="K24" t="s">
         <v>51</v>
+      </c>
+      <c r="L24" s="4" t="s">
+        <v>90</v>
       </c>
     </row>
     <row r="25" spans="1:12" x14ac:dyDescent="0.3">
@@ -1493,32 +1688,35 @@
       <c r="C25" s="4" t="s">
         <v>59</v>
       </c>
+      <c r="D25" t="s">
+        <v>13</v>
+      </c>
       <c r="E25" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F25" t="s">
-        <v>12</v>
+        <v>44</v>
       </c>
       <c r="G25" t="s">
-        <v>44</v>
-      </c>
-      <c r="H25" t="s">
         <v>22</v>
       </c>
-      <c r="I25">
+      <c r="H25">
         <v>3</v>
       </c>
+      <c r="I25" t="s">
+        <v>46</v>
+      </c>
       <c r="J25" t="s">
         <v>46</v>
       </c>
       <c r="K25" t="s">
-        <v>46</v>
-      </c>
-      <c r="L25" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="L25" s="4" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="26" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>9</v>
       </c>
@@ -1528,32 +1726,35 @@
       <c r="C26" s="4" t="s">
         <v>60</v>
       </c>
+      <c r="D26" t="s">
+        <v>12</v>
+      </c>
       <c r="E26" t="s">
         <v>12</v>
       </c>
       <c r="F26" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="G26" t="s">
-        <v>14</v>
-      </c>
-      <c r="H26" t="s">
         <v>15</v>
       </c>
+      <c r="H26">
+        <v>4</v>
+      </c>
       <c r="I26">
-        <v>4</v>
+        <v>3963</v>
       </c>
       <c r="J26">
-        <v>3963</v>
-      </c>
-      <c r="K26">
         <v>17748</v>
       </c>
-      <c r="L26" t="s">
+      <c r="K26" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="L26" s="4" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="27" spans="1:12" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>55</v>
       </c>
@@ -1563,32 +1764,35 @@
       <c r="C27" s="4" t="s">
         <v>61</v>
       </c>
+      <c r="D27" t="s">
+        <v>12</v>
+      </c>
       <c r="E27" t="s">
         <v>12</v>
       </c>
       <c r="F27" t="s">
-        <v>12</v>
+        <v>44</v>
       </c>
       <c r="G27" t="s">
-        <v>44</v>
-      </c>
-      <c r="H27" t="s">
         <v>22</v>
       </c>
+      <c r="H27">
+        <v>4</v>
+      </c>
       <c r="I27">
-        <v>4</v>
+        <v>1567</v>
       </c>
       <c r="J27">
-        <v>1567</v>
-      </c>
-      <c r="K27">
         <v>13320</v>
       </c>
-      <c r="L27" t="s">
+      <c r="K27" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="L27" s="4" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="28" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>9</v>
       </c>
@@ -1598,32 +1802,35 @@
       <c r="C28" s="4" t="s">
         <v>62</v>
       </c>
+      <c r="D28" t="s">
+        <v>12</v>
+      </c>
       <c r="E28" t="s">
         <v>12</v>
       </c>
       <c r="F28" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="G28" t="s">
-        <v>14</v>
-      </c>
-      <c r="H28" t="s">
         <v>15</v>
       </c>
+      <c r="H28">
+        <v>5</v>
+      </c>
       <c r="I28">
-        <v>5</v>
+        <v>5668</v>
       </c>
       <c r="J28">
-        <v>5668</v>
-      </c>
-      <c r="K28">
         <v>25664</v>
       </c>
-      <c r="L28" t="s">
+      <c r="K28" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="L28" s="4" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="29" spans="1:12" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>9</v>
       </c>
@@ -1633,29 +1840,32 @@
       <c r="C29" s="4" t="s">
         <v>63</v>
       </c>
+      <c r="D29" t="s">
+        <v>12</v>
+      </c>
       <c r="E29" t="s">
         <v>12</v>
       </c>
       <c r="F29" t="s">
-        <v>12</v>
+        <v>23</v>
       </c>
       <c r="G29" t="s">
-        <v>23</v>
-      </c>
-      <c r="H29" t="s">
         <v>15</v>
       </c>
+      <c r="H29">
+        <v>5</v>
+      </c>
       <c r="I29">
-        <v>5</v>
+        <v>808</v>
       </c>
       <c r="J29">
-        <v>808</v>
-      </c>
-      <c r="K29">
         <v>3372</v>
       </c>
-      <c r="L29" t="s">
+      <c r="K29" t="s">
         <v>75</v>
+      </c>
+      <c r="L29" s="4" t="s">
+        <v>94</v>
       </c>
     </row>
     <row r="30" spans="1:12" x14ac:dyDescent="0.3">
@@ -1668,32 +1878,35 @@
       <c r="C30" s="4" t="s">
         <v>64</v>
       </c>
+      <c r="D30" t="s">
+        <v>12</v>
+      </c>
       <c r="E30" t="s">
         <v>12</v>
       </c>
       <c r="F30" t="s">
-        <v>12</v>
+        <v>44</v>
       </c>
       <c r="G30" t="s">
-        <v>44</v>
-      </c>
-      <c r="H30" t="s">
         <v>22</v>
       </c>
-      <c r="I30">
+      <c r="H30">
         <v>4</v>
       </c>
+      <c r="I30" t="s">
+        <v>46</v>
+      </c>
       <c r="J30" t="s">
         <v>46</v>
       </c>
       <c r="K30" t="s">
-        <v>46</v>
-      </c>
-      <c r="L30" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="L30" s="4" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="31" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>72</v>
       </c>
@@ -1703,32 +1916,35 @@
       <c r="C31" s="4" t="s">
         <v>65</v>
       </c>
+      <c r="D31" t="s">
+        <v>12</v>
+      </c>
       <c r="E31" t="s">
         <v>12</v>
       </c>
       <c r="F31" t="s">
-        <v>12</v>
+        <v>44</v>
       </c>
       <c r="G31" t="s">
-        <v>44</v>
-      </c>
-      <c r="H31" t="s">
         <v>22</v>
       </c>
+      <c r="H31">
+        <v>4</v>
+      </c>
       <c r="I31">
-        <v>4</v>
+        <v>1029</v>
       </c>
       <c r="J31">
-        <v>1029</v>
-      </c>
-      <c r="K31">
         <v>8424</v>
       </c>
-      <c r="L31" t="s">
+      <c r="K31" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="L31" s="4" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="32" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>55</v>
       </c>
@@ -1738,29 +1954,32 @@
       <c r="C32" s="4" t="s">
         <v>66</v>
       </c>
+      <c r="D32" t="s">
+        <v>12</v>
+      </c>
       <c r="E32" t="s">
         <v>12</v>
       </c>
       <c r="F32" t="s">
-        <v>12</v>
+        <v>44</v>
       </c>
       <c r="G32" t="s">
-        <v>44</v>
-      </c>
-      <c r="H32" t="s">
         <v>22</v>
       </c>
+      <c r="H32">
+        <v>4</v>
+      </c>
       <c r="I32">
-        <v>4</v>
+        <v>457</v>
       </c>
       <c r="J32">
-        <v>457</v>
-      </c>
-      <c r="K32">
         <v>4793</v>
       </c>
-      <c r="L32" t="s">
+      <c r="K32" t="s">
         <v>24</v>
+      </c>
+      <c r="L32" s="4" t="s">
+        <v>96</v>
       </c>
     </row>
     <row r="33" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
@@ -1773,29 +1992,32 @@
       <c r="C33" s="4" t="s">
         <v>67</v>
       </c>
+      <c r="D33" t="s">
+        <v>45</v>
+      </c>
       <c r="E33" t="s">
-        <v>45</v>
+        <v>13</v>
       </c>
       <c r="F33" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="G33" t="s">
-        <v>14</v>
-      </c>
-      <c r="H33" t="s">
         <v>15</v>
       </c>
+      <c r="H33">
+        <v>5</v>
+      </c>
       <c r="I33">
-        <v>5</v>
+        <v>222</v>
       </c>
       <c r="J33">
-        <v>222</v>
-      </c>
-      <c r="K33">
         <v>888</v>
       </c>
-      <c r="L33" t="s">
+      <c r="K33" t="s">
         <v>49</v>
+      </c>
+      <c r="L33" s="4" t="s">
+        <v>97</v>
       </c>
     </row>
     <row r="34" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
@@ -1808,29 +2030,32 @@
       <c r="C34" s="4" t="s">
         <v>68</v>
       </c>
+      <c r="D34" t="s">
+        <v>45</v>
+      </c>
       <c r="E34" t="s">
         <v>45</v>
       </c>
       <c r="F34" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="G34" t="s">
-        <v>44</v>
-      </c>
-      <c r="H34" t="s">
         <v>22</v>
       </c>
-      <c r="I34">
+      <c r="H34">
         <v>4</v>
       </c>
+      <c r="I34" t="s">
+        <v>46</v>
+      </c>
       <c r="J34" t="s">
         <v>46</v>
       </c>
       <c r="K34" t="s">
-        <v>46</v>
-      </c>
-      <c r="L34" t="s">
         <v>49</v>
+      </c>
+      <c r="L34" s="4" t="s">
+        <v>98</v>
       </c>
     </row>
     <row r="35" spans="1:12" x14ac:dyDescent="0.3">
@@ -1843,29 +2068,32 @@
       <c r="C35" s="4" t="s">
         <v>69</v>
       </c>
+      <c r="D35" t="s">
+        <v>45</v>
+      </c>
       <c r="E35" t="s">
-        <v>45</v>
+        <v>12</v>
       </c>
       <c r="F35" t="s">
-        <v>12</v>
+        <v>23</v>
       </c>
       <c r="G35" t="s">
-        <v>23</v>
-      </c>
-      <c r="H35" t="s">
         <v>15</v>
       </c>
+      <c r="H35">
+        <v>5</v>
+      </c>
       <c r="I35">
-        <v>5</v>
+        <v>377</v>
       </c>
       <c r="J35">
-        <v>377</v>
-      </c>
-      <c r="K35">
         <v>1557</v>
       </c>
-      <c r="L35" t="s">
+      <c r="K35" t="s">
         <v>49</v>
+      </c>
+      <c r="L35" s="4" t="s">
+        <v>97</v>
       </c>
     </row>
     <row r="36" spans="1:12" x14ac:dyDescent="0.3">
@@ -1878,29 +2106,32 @@
       <c r="C36" s="4" t="s">
         <v>70</v>
       </c>
+      <c r="D36" t="s">
+        <v>45</v>
+      </c>
       <c r="E36" t="s">
-        <v>45</v>
+        <v>12</v>
       </c>
       <c r="F36" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="G36" t="s">
-        <v>14</v>
-      </c>
-      <c r="H36" t="s">
         <v>15</v>
       </c>
-      <c r="I36">
+      <c r="H36">
         <v>4</v>
       </c>
+      <c r="I36" t="s">
+        <v>46</v>
+      </c>
       <c r="J36" t="s">
         <v>46</v>
       </c>
       <c r="K36" t="s">
-        <v>46</v>
-      </c>
-      <c r="L36" t="s">
         <v>49</v>
+      </c>
+      <c r="L36" s="4" t="s">
+        <v>99</v>
       </c>
     </row>
     <row r="37" spans="1:12" x14ac:dyDescent="0.3">
@@ -1913,44 +2144,47 @@
       <c r="C37" s="4" t="s">
         <v>71</v>
       </c>
+      <c r="D37" t="s">
+        <v>45</v>
+      </c>
       <c r="E37" t="s">
-        <v>45</v>
+        <v>12</v>
       </c>
       <c r="F37" t="s">
-        <v>12</v>
+        <v>23</v>
       </c>
       <c r="G37" t="s">
-        <v>23</v>
-      </c>
-      <c r="H37" t="s">
         <v>15</v>
       </c>
+      <c r="H37">
+        <v>5</v>
+      </c>
       <c r="I37">
-        <v>5</v>
+        <v>1406</v>
       </c>
       <c r="J37">
-        <v>1406</v>
-      </c>
-      <c r="K37">
         <v>6434</v>
       </c>
-      <c r="L37" t="s">
+      <c r="K37" t="s">
         <v>49</v>
+      </c>
+      <c r="L37" s="4" t="s">
+        <v>100</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="12">
-    <mergeCell ref="N1:N2"/>
-    <mergeCell ref="J1:K1"/>
+    <mergeCell ref="M1:M2"/>
+    <mergeCell ref="I1:J1"/>
+    <mergeCell ref="F1:F2"/>
     <mergeCell ref="G1:G2"/>
     <mergeCell ref="H1:H2"/>
-    <mergeCell ref="I1:I2"/>
+    <mergeCell ref="K1:K2"/>
     <mergeCell ref="L1:L2"/>
-    <mergeCell ref="M1:M2"/>
-    <mergeCell ref="E1:F1"/>
+    <mergeCell ref="D1:E1"/>
     <mergeCell ref="A1:A2"/>
     <mergeCell ref="C1:C2"/>
-    <mergeCell ref="D1:D2"/>
+    <mergeCell ref="N1:N2"/>
     <mergeCell ref="B1:B2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
finish southcoast CU summary
</commit_message>
<xml_diff>
--- a/data/southcoastCUs.xlsx
+++ b/data/southcoastCUs.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="364" uniqueCount="116">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="416" uniqueCount="168">
   <si>
     <t>Region</t>
   </si>
@@ -329,49 +329,205 @@
     <t>Low quality data, but may be abundant</t>
   </si>
   <si>
-    <t>Baker, Bridge, Chilako, Chilcotin, Endako, Narcosli, Naver, West Road, Baezaeko, Cottonwood, Horsefly, Nazko</t>
-  </si>
-  <si>
     <t>Current surveys may underestimate abundance due to large watershed size</t>
   </si>
   <si>
-    <t>Adams, Little, South Thompson, Thompson</t>
-  </si>
-  <si>
     <t>May not be a distinct CU (part of Middle Shuswap)</t>
   </si>
   <si>
-    <t>Bessette, Duteau</t>
-  </si>
-  <si>
     <t>Relatively little basic information for this CU; absolute abundance likely much greater than relative index</t>
   </si>
   <si>
-    <t>Blue, Finn</t>
-  </si>
-  <si>
     <t>Okanagan</t>
   </si>
   <si>
-    <t>Barriere, Lemieux, Mahood, Clearwater, Raft</t>
-  </si>
-  <si>
     <t>Represents succesful recolonization from Lower Shuswap</t>
   </si>
   <si>
-    <t>Adams (upper)</t>
-  </si>
-  <si>
     <t>No havitat based benchmarks and low quality data</t>
   </si>
   <si>
-    <t>Big Silver</t>
-  </si>
-  <si>
     <t>One of the largest and most intensively studied populations; status may be corrupted by hatchery contributions</t>
   </si>
   <si>
     <t>Harrison River</t>
+  </si>
+  <si>
+    <t>Extensive NuSEDS issues</t>
+  </si>
+  <si>
+    <t>Pitt River</t>
+  </si>
+  <si>
+    <t>Despite assessment relative index is still within range of historical</t>
+  </si>
+  <si>
+    <t>Portage Creek</t>
+  </si>
+  <si>
+    <t>Sites may not be representative considering large spatial area</t>
+  </si>
+  <si>
+    <t>No data stream for wild sites, but hatchery releases halted in 2004</t>
+  </si>
+  <si>
+    <t>Spawner abundances generally low and no data stream for wild sites (likely high ppn of hatchery spawners); may not be a viable population and just sustained by strays</t>
+  </si>
+  <si>
+    <t>Many rivers with persistent pops but only one (enahnced) spawner abundance TS; no data stream for wild Cus; unclear what enhancement objectives are (i.e. need either exploitation rates or contribution to spawner abundance)</t>
+  </si>
+  <si>
+    <t>Marble (East, Keith, Klaskish, Mahatta, Washlawlis, Goodspeed, Cayeghle, Benson, Utluh)</t>
+  </si>
+  <si>
+    <t>Goldstream (Tod)</t>
+  </si>
+  <si>
+    <t>Birkenhead (Green)</t>
+  </si>
+  <si>
+    <t>Kuzkwa, Pinchi, Cariboo, Chilko, Nechako, Quesnel (Elkin, Kazchek, Mitchell, Ormond, Seton, Stellako, Taseko, Stuart, Middle, Tachie)</t>
+  </si>
+  <si>
+    <t>Big Silver (Cogburn, Douglas, Lillooet, Sloquet, Tipella, Chilliwack)</t>
+  </si>
+  <si>
+    <t>Upper Adams</t>
+  </si>
+  <si>
+    <t>Barriere, Lemieux, Mahood, Clearwater, Raft (Mann, North Thompson)</t>
+  </si>
+  <si>
+    <t>Blue, Finn (Albreda, Lyon, Mad)</t>
+  </si>
+  <si>
+    <t>Bessette, Duteau (Creighton, Harris)</t>
+  </si>
+  <si>
+    <t>Adams, Little, South Thompson, Thompson (Adams River channel)</t>
+  </si>
+  <si>
+    <t>Baker, Bridge, Chilako, Chilcotin, Endako, Narcosli, Naver, West Road, Baezaeko, Cottonwood, Horsefly, Nazko (Upper Cariboo, Churn, Driftwood, Stein, Taseko, Ahbau, Lightning, McKinley, Shovel, Swift, Yalakom)</t>
+  </si>
+  <si>
+    <t>EU data quality is very high, but no data stream for wild sites</t>
+  </si>
+  <si>
+    <t>Cowichan (Koksilah, Mesachie, patricia, Robertson, Shaw)</t>
+  </si>
+  <si>
+    <t>All sites likely highly enhanced, including contributions from other EUs; extremely high human pop density, but limited information on biology or status; no wild site data stream</t>
+  </si>
+  <si>
+    <t>Little Campbell River (Serpentine, Nicomeki)</t>
+  </si>
+  <si>
+    <t>Small with extensive restoriation activity; no wild site data stream</t>
+  </si>
+  <si>
+    <t>Maria Slough</t>
+  </si>
+  <si>
+    <t>No wild site data stream; no spawner abundance calibration; no exploitation rate estimates</t>
+  </si>
+  <si>
+    <t>Nanaimo (Chemainus, Haslam, Napoleon)</t>
+  </si>
+  <si>
+    <t>No wild site data stream; despite high enhancement levels and reduced fishing mortality little evidence of recovery; cyclicity may indicate issues with age data</t>
+  </si>
+  <si>
+    <t>Shuswap lower and middle (Wap)</t>
+  </si>
+  <si>
+    <t>No wild data stream; poor marine survival and high exploitation rate suggests the CU would collapse if there was no hatchery production</t>
+  </si>
+  <si>
+    <t>Puntledge (Nanaimo, First Nanaimo Lake)</t>
+  </si>
+  <si>
+    <t>No wild data stream; most rivers have received some enhancement; hatchery production likely exceeds spawning habitat; extremely low marine survival; good enhanced production because habitat fully seeded</t>
+  </si>
+  <si>
+    <t>Englishman, Little Qualicum, Puntledge, Qualicum (Simms, Willow, Tsable, Oyster, Morrison, Tsolum)</t>
+  </si>
+  <si>
+    <t>Enitrely derived from Harrison Fall Chinook; no wild data stream; EU is healthy (good survival, exploitation rate and abundance)</t>
+  </si>
+  <si>
+    <t>Chilliwack, Vedder</t>
+  </si>
+  <si>
+    <t>Relative index because known wild stream doesn't contribute to data (due to water clarity) but contributes considerably to abundance; stream-type w/ short generation, small body size; dramatic declines are real; ppn of enhanced fish varies widely; large declines in hatchery releases; low and variable marine survival; anomalously high recent exploitation rates</t>
+  </si>
+  <si>
+    <t>Bonaparte, Deadman, Nicola, Coldwater, Spius (Louis, Coldwater upper, Nicola upper, Spius)</t>
+  </si>
+  <si>
+    <t>Large number of sites span a considerable area w/ diff. habitats; EU dominates abundance; variable quality; notable straying; data from 2 of 21 wild sites likely not rep.; hatchery/wild TS out of synch; terminal closures only apply to monitored sites; considerable Alaskan harvest; TU could be green based on EU or red based on CU</t>
+  </si>
+  <si>
+    <t>Megin, Moyeha, Bedwell, Nahmint, Nitinat, San Juan, Sarita, Somass-Sproat-GC, Sooke, Tranquil (Carnation, Caycuse, China, Coeur D'alene, Coleman, Cous, Effinham, Franklin, Ice, Klanawa, Macktush, Mercantile, Smith, Sydney, Thornton, Toquart, Ayum, Charters, Clayoquot, De Mamial, Deer, Drinkwater, Harris, Kennedy Lake, Kennedy River, Lens, Little Toquart, Muriel, Renfrew, Rocky, Sand, Clemens, Stamp)</t>
+  </si>
+  <si>
+    <t>Enhancement likely minimal; abs. abundance likely amber, but trend is clearly downward; lack of survival/ER data because Dome Creek CWT terminated</t>
+  </si>
+  <si>
+    <t>Captain, Fontoniko, Tete Jaune, Goat, Holliday, Holmes, Horsey, Ice, McKale, Morkill, Nevin, Salmon, Small, Swift, Torpy, Twin Creeks, Walker, Wansa, Bad, Bowron, Indianpoint, Seebach, Slim, Willow, Dome (Haggen, McGregor, Ptarmigan, Robson, Snowshoe, Forgetmenot, Herrick, Humbug, Otter, Spakwaniko, Sus)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Spawner abundance ~even H and W; extensive life history variation due to difficult hydrology; rel. abundance and short-term trend are red, but visual estimates may be biased low; sites may not be representative; hatchery releases are relatively small and declining </t>
+  </si>
+  <si>
+    <t>Eagle, Salmon (Scotch, Seymour)</t>
+  </si>
+  <si>
+    <t>Hatchery contributions increasing; no habitat based estimate of abundance; main life history varies among sites (ocean-type at lower elevations, stream-type further up); relatively few sites are assessed but enhanced may be trending up</t>
+  </si>
+  <si>
+    <t>Kingcome, Wakeman, Phillips (Apple, Franklin, Fulmore, Heydon, Kakweiken, Kwalate, Sim, Southgate, Stafford, Teaquahan, Warner Bay, Orford, Ahnuhati)</t>
+  </si>
+  <si>
+    <t>Dominated by hatchery and some outside CU straying; borderline data deficient; hatchery production provides stable harvest</t>
+  </si>
+  <si>
+    <t>Adam, Campbell, Quinsam (Salmon, Amor De Cosmos, Cluxewe, Menzies, Mohun, Tsitika, White, Kokish, Quatse, Nimpkish, Eve)</t>
+  </si>
+  <si>
+    <t>Dominated by hatchery (one enahnced stock drives majority of trends); minimal data stream for wild stocks; widely distributed among rivers</t>
+  </si>
+  <si>
+    <t>Kaouk, Tahsish, Artlish, Leiner, Burman, Conuma, Tahsis, Zeballos (Amai, Battle Bay, Brodick, Canton, Chamiss, Chum, Clanninick, Easy, Eliza, Espinosa, Hoiss, Houston, Jacklah, Kashutl, Kauwinch, Kleeptee, Little Zebalos, Malksope, Mamat, Marvinas, McKay Cove, Narrowgut, Nasparti, Ouokinsh, park, Power, Silverado, Tsowwin, Mooyah, Gold, Sucwoa, Tlupana, Deserted, Oktwanch, Silburn, Muchalat)</t>
+  </si>
+  <si>
+    <t>Long time series of uncertain historical spawner abundance; water clarity issues</t>
+  </si>
+  <si>
+    <t>(Anderson, Nahatlatch)</t>
+  </si>
+  <si>
+    <t>Highly variable data quality among large number of sites</t>
+  </si>
+  <si>
+    <t>(Brem, Brothers, Indian, Lynn, Quatam, Richards, Skwawka, Toba, Tzoonie, Seymour, Theodosia, Squamish, Branch 100, Brem, Chuk-chuk, July, Klite, Little Toba, Mamquam, Mashiter, Shovelnose, Spring, Ashlu, Cheakamus, Tenderfoot)</t>
+  </si>
+  <si>
+    <t>Large glacially turbid system; uncertain historical data quality</t>
+  </si>
+  <si>
+    <t>Unique and very small</t>
+  </si>
+  <si>
+    <t>(Nanaimo River upper)</t>
+  </si>
+  <si>
+    <t>(Homathko, Cumsack)</t>
+  </si>
+  <si>
+    <t>Wild sites only, but not affiliated with any regular survey; may be rel. abundant based on short-term fishwheel project</t>
+  </si>
+  <si>
+    <t>(Klinaklini, Devereux)</t>
   </si>
 </sst>
 </file>
@@ -417,15 +573,15 @@
   </cellStyleXfs>
   <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -713,98 +869,98 @@
   <dimension ref="A1:N37"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="L8" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="1" topLeftCell="M33" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="M12" sqref="M12"/>
+      <selection pane="bottomRight" activeCell="N37" sqref="N37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" width="12.109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="29" style="4" customWidth="1"/>
+    <col min="3" max="3" width="29" style="2" customWidth="1"/>
     <col min="4" max="4" width="7.88671875" customWidth="1"/>
     <col min="5" max="5" width="8.5546875" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="8.21875" customWidth="1"/>
     <col min="7" max="7" width="8.44140625" customWidth="1"/>
     <col min="10" max="10" width="10.88671875" customWidth="1"/>
-    <col min="12" max="12" width="41.77734375" style="4" customWidth="1"/>
-    <col min="13" max="13" width="32" style="4" customWidth="1"/>
-    <col min="14" max="14" width="32.5546875" style="4" customWidth="1"/>
+    <col min="12" max="12" width="41.77734375" style="2" customWidth="1"/>
+    <col min="13" max="13" width="55.109375" style="2" customWidth="1"/>
+    <col min="14" max="14" width="38.33203125" style="2" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1"/>
-      <c r="F1" s="2" t="s">
+      <c r="E1" s="4"/>
+      <c r="F1" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="G1" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="H1" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="I1" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="J1" s="2"/>
-      <c r="K1" s="1" t="s">
+      <c r="J1" s="5"/>
+      <c r="K1" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="L1" s="2" t="s">
+      <c r="L1" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="M1" s="2" t="s">
+      <c r="M1" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="N1" s="2" t="s">
+      <c r="N1" s="5" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A2" s="1"/>
-      <c r="B2" s="1"/>
-      <c r="C2" s="2"/>
-      <c r="D2" s="3" t="s">
+      <c r="A2" s="4"/>
+      <c r="B2" s="4"/>
+      <c r="C2" s="5"/>
+      <c r="D2" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="E2" s="3" t="s">
+      <c r="E2" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="F2" s="2"/>
-      <c r="G2" s="2"/>
-      <c r="H2" s="2"/>
-      <c r="I2" s="5" t="s">
+      <c r="F2" s="5"/>
+      <c r="G2" s="5"/>
+      <c r="H2" s="5"/>
+      <c r="I2" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="J2" s="5" t="s">
+      <c r="J2" s="3" t="s">
         <v>76</v>
       </c>
-      <c r="K2" s="1"/>
-      <c r="L2" s="2"/>
-      <c r="M2" s="2"/>
-      <c r="N2" s="2"/>
-    </row>
-    <row r="3" spans="1:14" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="K2" s="4"/>
+      <c r="L2" s="5"/>
+      <c r="M2" s="5"/>
+      <c r="N2" s="5"/>
+    </row>
+    <row r="3" spans="1:14" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>9</v>
       </c>
       <c r="B3" t="s">
         <v>10</v>
       </c>
-      <c r="C3" s="4" t="s">
+      <c r="C3" s="2" t="s">
         <v>11</v>
       </c>
       <c r="D3" t="s">
@@ -831,21 +987,21 @@
       <c r="K3" t="s">
         <v>24</v>
       </c>
-      <c r="L3" s="4" t="s">
+      <c r="L3" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="N3" s="4" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="4" spans="1:14" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="N3" s="2" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>9</v>
       </c>
       <c r="B4" t="s">
         <v>20</v>
       </c>
-      <c r="C4" s="4" t="s">
+      <c r="C4" s="2" t="s">
         <v>21</v>
       </c>
       <c r="D4" t="s">
@@ -869,14 +1025,14 @@
       <c r="K4" t="s">
         <v>25</v>
       </c>
-      <c r="L4" s="4" t="s">
+      <c r="L4" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="M4" s="4" t="s">
-        <v>102</v>
-      </c>
-      <c r="N4" s="4" t="s">
-        <v>103</v>
+      <c r="M4" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="N4" s="2" t="s">
+        <v>126</v>
       </c>
     </row>
     <row r="5" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
@@ -886,7 +1042,7 @@
       <c r="B5" t="s">
         <v>20</v>
       </c>
-      <c r="C5" s="4" t="s">
+      <c r="C5" s="2" t="s">
         <v>26</v>
       </c>
       <c r="D5" t="s">
@@ -913,14 +1069,14 @@
       <c r="K5" t="s">
         <v>24</v>
       </c>
-      <c r="L5" s="4" t="s">
+      <c r="L5" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="M5" s="4" t="s">
-        <v>104</v>
-      </c>
-      <c r="N5" s="4" t="s">
-        <v>105</v>
+      <c r="M5" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="N5" s="2" t="s">
+        <v>125</v>
       </c>
     </row>
     <row r="6" spans="1:14" ht="43.2" x14ac:dyDescent="0.3">
@@ -930,7 +1086,7 @@
       <c r="B6" t="s">
         <v>20</v>
       </c>
-      <c r="C6" s="4" t="s">
+      <c r="C6" s="2" t="s">
         <v>27</v>
       </c>
       <c r="D6" t="s">
@@ -957,14 +1113,14 @@
       <c r="K6" t="s">
         <v>24</v>
       </c>
-      <c r="L6" s="4" t="s">
+      <c r="L6" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="M6" s="4" t="s">
-        <v>106</v>
-      </c>
-      <c r="N6" s="4" t="s">
-        <v>107</v>
+      <c r="M6" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="N6" s="2" t="s">
+        <v>124</v>
       </c>
     </row>
     <row r="7" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
@@ -974,7 +1130,7 @@
       <c r="B7" t="s">
         <v>46</v>
       </c>
-      <c r="C7" s="4" t="s">
+      <c r="C7" s="2" t="s">
         <v>31</v>
       </c>
       <c r="D7" t="s">
@@ -1001,24 +1157,24 @@
       <c r="K7" t="s">
         <v>24</v>
       </c>
-      <c r="L7" s="4" t="s">
+      <c r="L7" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="M7" s="4" t="s">
+      <c r="M7" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="N7" s="4" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="8" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="N7" s="2" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>9</v>
       </c>
       <c r="B8" t="s">
         <v>20</v>
       </c>
-      <c r="C8" s="4" t="s">
+      <c r="C8" s="2" t="s">
         <v>32</v>
       </c>
       <c r="D8" t="s">
@@ -1045,11 +1201,11 @@
       <c r="K8" t="s">
         <v>24</v>
       </c>
-      <c r="L8" s="4" t="s">
+      <c r="L8" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="N8" s="4" t="s">
-        <v>109</v>
+      <c r="N8" s="2" t="s">
+        <v>123</v>
       </c>
     </row>
     <row r="9" spans="1:14" ht="43.2" x14ac:dyDescent="0.3">
@@ -1059,7 +1215,7 @@
       <c r="B9" t="s">
         <v>20</v>
       </c>
-      <c r="C9" s="4" t="s">
+      <c r="C9" s="2" t="s">
         <v>33</v>
       </c>
       <c r="D9" t="s">
@@ -1086,14 +1242,14 @@
       <c r="K9" t="s">
         <v>49</v>
       </c>
-      <c r="L9" s="4" t="s">
+      <c r="L9" s="2" t="s">
         <v>84</v>
       </c>
-      <c r="M9" s="4" t="s">
-        <v>110</v>
-      </c>
-      <c r="N9" s="4" t="s">
-        <v>111</v>
+      <c r="M9" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="N9" s="2" t="s">
+        <v>122</v>
       </c>
     </row>
     <row r="10" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
@@ -1103,7 +1259,7 @@
       <c r="B10" t="s">
         <v>52</v>
       </c>
-      <c r="C10" s="4" t="s">
+      <c r="C10" s="2" t="s">
         <v>34</v>
       </c>
       <c r="D10" t="s">
@@ -1130,14 +1286,14 @@
       <c r="K10" t="s">
         <v>49</v>
       </c>
-      <c r="L10" s="4" t="s">
+      <c r="L10" s="2" t="s">
         <v>85</v>
       </c>
-      <c r="M10" s="4" t="s">
-        <v>112</v>
-      </c>
-      <c r="N10" s="4" t="s">
-        <v>113</v>
+      <c r="M10" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="N10" s="2" t="s">
+        <v>121</v>
       </c>
     </row>
     <row r="11" spans="1:14" ht="57.6" x14ac:dyDescent="0.3">
@@ -1147,7 +1303,7 @@
       <c r="B11" t="s">
         <v>52</v>
       </c>
-      <c r="C11" s="4" t="s">
+      <c r="C11" s="2" t="s">
         <v>35</v>
       </c>
       <c r="D11" t="s">
@@ -1174,14 +1330,14 @@
       <c r="K11" t="s">
         <v>25</v>
       </c>
-      <c r="L11" s="4" t="s">
+      <c r="L11" s="2" t="s">
         <v>86</v>
       </c>
-      <c r="M11" s="4" t="s">
-        <v>114</v>
-      </c>
-      <c r="N11" s="4" t="s">
-        <v>115</v>
+      <c r="M11" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="N11" s="2" t="s">
+        <v>108</v>
       </c>
     </row>
     <row r="12" spans="1:14" ht="43.2" x14ac:dyDescent="0.3">
@@ -1191,7 +1347,7 @@
       <c r="B12" t="s">
         <v>52</v>
       </c>
-      <c r="C12" s="4" t="s">
+      <c r="C12" s="2" t="s">
         <v>36</v>
       </c>
       <c r="D12" t="s">
@@ -1218,8 +1374,14 @@
       <c r="K12" t="s">
         <v>49</v>
       </c>
-      <c r="L12" s="4" t="s">
+      <c r="L12" s="2" t="s">
         <v>87</v>
+      </c>
+      <c r="M12" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="N12" s="2" t="s">
+        <v>110</v>
       </c>
     </row>
     <row r="13" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
@@ -1229,7 +1391,7 @@
       <c r="B13" t="s">
         <v>53</v>
       </c>
-      <c r="C13" s="4" t="s">
+      <c r="C13" s="2" t="s">
         <v>37</v>
       </c>
       <c r="D13" t="s">
@@ -1256,18 +1418,24 @@
       <c r="K13" t="s">
         <v>24</v>
       </c>
-      <c r="L13" s="4" t="s">
+      <c r="L13" s="2" t="s">
         <v>88</v>
       </c>
-    </row>
-    <row r="14" spans="1:14" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="M13" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="N13" s="2" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>9</v>
       </c>
       <c r="B14" t="s">
         <v>53</v>
       </c>
-      <c r="C14" s="4" t="s">
+      <c r="C14" s="2" t="s">
         <v>38</v>
       </c>
       <c r="D14" t="s">
@@ -1294,18 +1462,24 @@
       <c r="K14" t="s">
         <v>50</v>
       </c>
-      <c r="L14" s="4" t="s">
+      <c r="L14" s="2" t="s">
         <v>89</v>
       </c>
-    </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="M14" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="N14" s="2" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>9</v>
       </c>
       <c r="B15" t="s">
         <v>53</v>
       </c>
-      <c r="C15" s="4" t="s">
+      <c r="C15" s="2" t="s">
         <v>39</v>
       </c>
       <c r="D15" t="s">
@@ -1332,18 +1506,24 @@
       <c r="K15" t="s">
         <v>51</v>
       </c>
-      <c r="L15" s="4" t="s">
+      <c r="L15" s="2" t="s">
         <v>90</v>
       </c>
-    </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="M15" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="N15" s="2" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>72</v>
       </c>
       <c r="B16" t="s">
         <v>54</v>
       </c>
-      <c r="C16" s="4" t="s">
+      <c r="C16" s="2" t="s">
         <v>40</v>
       </c>
       <c r="D16" t="s">
@@ -1370,18 +1550,24 @@
       <c r="K16" t="s">
         <v>51</v>
       </c>
-      <c r="L16" s="4" t="s">
+      <c r="L16" s="2" t="s">
         <v>90</v>
       </c>
-    </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M16" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="N16" s="2" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="17" spans="1:14" ht="72" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>55</v>
       </c>
       <c r="B17" t="s">
         <v>46</v>
       </c>
-      <c r="C17" s="4" t="s">
+      <c r="C17" s="2" t="s">
         <v>48</v>
       </c>
       <c r="D17" t="s">
@@ -1408,18 +1594,24 @@
       <c r="K17" t="s">
         <v>51</v>
       </c>
-      <c r="L17" s="4" t="s">
+      <c r="L17" s="2" t="s">
         <v>90</v>
       </c>
-    </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M17" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="N17" s="2" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="18" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>54</v>
       </c>
       <c r="B18" t="s">
         <v>54</v>
       </c>
-      <c r="C18" s="4" t="s">
+      <c r="C18" s="2" t="s">
         <v>47</v>
       </c>
       <c r="D18" t="s">
@@ -1446,18 +1638,24 @@
       <c r="K18" t="s">
         <v>51</v>
       </c>
-      <c r="L18" s="4" t="s">
+      <c r="L18" s="2" t="s">
         <v>90</v>
       </c>
-    </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M18" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="N18" s="2" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="19" spans="1:14" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>73</v>
       </c>
       <c r="B19" t="s">
         <v>54</v>
       </c>
-      <c r="C19" s="4" t="s">
+      <c r="C19" s="2" t="s">
         <v>41</v>
       </c>
       <c r="D19" t="s">
@@ -1484,18 +1682,24 @@
       <c r="K19" t="s">
         <v>51</v>
       </c>
-      <c r="L19" s="4" t="s">
+      <c r="L19" s="2" t="s">
         <v>90</v>
       </c>
-    </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M19" s="2" t="s">
+        <v>130</v>
+      </c>
+      <c r="N19" s="2" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="20" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>9</v>
       </c>
       <c r="B20" t="s">
         <v>52</v>
       </c>
-      <c r="C20" s="4" t="s">
+      <c r="C20" s="2" t="s">
         <v>42</v>
       </c>
       <c r="D20" t="s">
@@ -1522,18 +1726,24 @@
       <c r="K20" t="s">
         <v>51</v>
       </c>
-      <c r="L20" s="4" t="s">
+      <c r="L20" s="2" t="s">
         <v>90</v>
       </c>
-    </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M20" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="N20" s="2" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="21" spans="1:14" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>72</v>
       </c>
       <c r="B21" t="s">
         <v>54</v>
       </c>
-      <c r="C21" s="4" t="s">
+      <c r="C21" s="2" t="s">
         <v>43</v>
       </c>
       <c r="D21" t="s">
@@ -1560,18 +1770,24 @@
       <c r="K21" t="s">
         <v>51</v>
       </c>
-      <c r="L21" s="4" t="s">
+      <c r="L21" s="2" t="s">
         <v>90</v>
       </c>
-    </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M21" s="2" t="s">
+        <v>134</v>
+      </c>
+      <c r="N21" s="2" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="22" spans="1:14" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>9</v>
       </c>
       <c r="B22" t="s">
         <v>20</v>
       </c>
-      <c r="C22" s="4" t="s">
+      <c r="C22" s="2" t="s">
         <v>56</v>
       </c>
       <c r="D22" t="s">
@@ -1598,18 +1814,24 @@
       <c r="K22" t="s">
         <v>51</v>
       </c>
-      <c r="L22" s="4" t="s">
+      <c r="L22" s="2" t="s">
         <v>90</v>
       </c>
-    </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M22" s="2" t="s">
+        <v>136</v>
+      </c>
+      <c r="N22" s="2" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="23" spans="1:14" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>72</v>
       </c>
       <c r="B23" t="s">
         <v>54</v>
       </c>
-      <c r="C23" s="4" t="s">
+      <c r="C23" s="2" t="s">
         <v>57</v>
       </c>
       <c r="D23" t="s">
@@ -1636,18 +1858,24 @@
       <c r="K23" t="s">
         <v>51</v>
       </c>
-      <c r="L23" s="4" t="s">
+      <c r="L23" s="2" t="s">
         <v>90</v>
       </c>
-    </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M23" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="N23" s="2" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="24" spans="1:14" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>72</v>
       </c>
       <c r="B24" t="s">
         <v>54</v>
       </c>
-      <c r="C24" s="4" t="s">
+      <c r="C24" s="2" t="s">
         <v>58</v>
       </c>
       <c r="D24" t="s">
@@ -1674,18 +1902,24 @@
       <c r="K24" t="s">
         <v>51</v>
       </c>
-      <c r="L24" s="4" t="s">
+      <c r="L24" s="2" t="s">
         <v>90</v>
       </c>
-    </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M24" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="N24" s="2" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="25" spans="1:14" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>9</v>
       </c>
       <c r="B25" t="s">
         <v>52</v>
       </c>
-      <c r="C25" s="4" t="s">
+      <c r="C25" s="2" t="s">
         <v>59</v>
       </c>
       <c r="D25" t="s">
@@ -1712,18 +1946,24 @@
       <c r="K25" t="s">
         <v>51</v>
       </c>
-      <c r="L25" s="4" t="s">
+      <c r="L25" s="2" t="s">
         <v>90</v>
       </c>
-    </row>
-    <row r="26" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="M25" s="2" t="s">
+        <v>142</v>
+      </c>
+      <c r="N25" s="2" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="26" spans="1:14" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>9</v>
       </c>
       <c r="B26" t="s">
         <v>20</v>
       </c>
-      <c r="C26" s="4" t="s">
+      <c r="C26" s="2" t="s">
         <v>60</v>
       </c>
       <c r="D26" t="s">
@@ -1750,18 +1990,24 @@
       <c r="K26" t="s">
         <v>24</v>
       </c>
-      <c r="L26" s="4" t="s">
+      <c r="L26" s="2" t="s">
         <v>91</v>
       </c>
-    </row>
-    <row r="27" spans="1:12" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="M26" s="2" t="s">
+        <v>144</v>
+      </c>
+      <c r="N26" s="2" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="27" spans="1:14" ht="172.8" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>55</v>
       </c>
       <c r="B27" t="s">
         <v>46</v>
       </c>
-      <c r="C27" s="4" t="s">
+      <c r="C27" s="2" t="s">
         <v>61</v>
       </c>
       <c r="D27" t="s">
@@ -1788,18 +2034,24 @@
       <c r="K27" t="s">
         <v>24</v>
       </c>
-      <c r="L27" s="4" t="s">
+      <c r="L27" s="2" t="s">
         <v>92</v>
       </c>
-    </row>
-    <row r="28" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="M27" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="N27" s="2" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="28" spans="1:14" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>9</v>
       </c>
       <c r="B28" t="s">
         <v>53</v>
       </c>
-      <c r="C28" s="4" t="s">
+      <c r="C28" s="2" t="s">
         <v>62</v>
       </c>
       <c r="D28" t="s">
@@ -1826,18 +2078,24 @@
       <c r="K28" t="s">
         <v>24</v>
       </c>
-      <c r="L28" s="4" t="s">
+      <c r="L28" s="2" t="s">
         <v>93</v>
       </c>
-    </row>
-    <row r="29" spans="1:12" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="M28" s="2" t="s">
+        <v>148</v>
+      </c>
+      <c r="N28" s="2" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="29" spans="1:14" ht="72" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>9</v>
       </c>
       <c r="B29" t="s">
         <v>20</v>
       </c>
-      <c r="C29" s="4" t="s">
+      <c r="C29" s="2" t="s">
         <v>63</v>
       </c>
       <c r="D29" t="s">
@@ -1864,18 +2122,24 @@
       <c r="K29" t="s">
         <v>75</v>
       </c>
-      <c r="L29" s="4" t="s">
+      <c r="L29" s="2" t="s">
         <v>94</v>
       </c>
-    </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M29" s="2" t="s">
+        <v>150</v>
+      </c>
+      <c r="N29" s="2" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="30" spans="1:14" ht="72" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>73</v>
       </c>
       <c r="B30" t="s">
         <v>74</v>
       </c>
-      <c r="C30" s="4" t="s">
+      <c r="C30" s="2" t="s">
         <v>64</v>
       </c>
       <c r="D30" t="s">
@@ -1902,18 +2166,24 @@
       <c r="K30" t="s">
         <v>49</v>
       </c>
-      <c r="L30" s="4" t="s">
+      <c r="L30" s="2" t="s">
         <v>95</v>
       </c>
-    </row>
-    <row r="31" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="M30" s="2" t="s">
+        <v>152</v>
+      </c>
+      <c r="N30" s="2" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="31" spans="1:14" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>72</v>
       </c>
       <c r="B31" t="s">
         <v>74</v>
       </c>
-      <c r="C31" s="4" t="s">
+      <c r="C31" s="2" t="s">
         <v>65</v>
       </c>
       <c r="D31" t="s">
@@ -1940,18 +2210,24 @@
       <c r="K31" t="s">
         <v>24</v>
       </c>
-      <c r="L31" s="4" t="s">
+      <c r="L31" s="2" t="s">
         <v>96</v>
       </c>
-    </row>
-    <row r="32" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="M31" s="2" t="s">
+        <v>154</v>
+      </c>
+      <c r="N31" s="2" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="32" spans="1:14" ht="172.8" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>55</v>
       </c>
       <c r="B32" t="s">
         <v>46</v>
       </c>
-      <c r="C32" s="4" t="s">
+      <c r="C32" s="2" t="s">
         <v>66</v>
       </c>
       <c r="D32" t="s">
@@ -1978,18 +2254,24 @@
       <c r="K32" t="s">
         <v>24</v>
       </c>
-      <c r="L32" s="4" t="s">
+      <c r="L32" s="2" t="s">
         <v>96</v>
       </c>
-    </row>
-    <row r="33" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="M32" s="2" t="s">
+        <v>156</v>
+      </c>
+      <c r="N32" s="2" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="33" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>9</v>
       </c>
       <c r="B33" t="s">
         <v>53</v>
       </c>
-      <c r="C33" s="4" t="s">
+      <c r="C33" s="2" t="s">
         <v>67</v>
       </c>
       <c r="D33" t="s">
@@ -2016,18 +2298,24 @@
       <c r="K33" t="s">
         <v>49</v>
       </c>
-      <c r="L33" s="4" t="s">
+      <c r="L33" s="2" t="s">
         <v>97</v>
       </c>
-    </row>
-    <row r="34" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="M33" s="2" t="s">
+        <v>158</v>
+      </c>
+      <c r="N33" s="2" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="34" spans="1:14" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>73</v>
       </c>
       <c r="B34" t="s">
         <v>54</v>
       </c>
-      <c r="C34" s="4" t="s">
+      <c r="C34" s="2" t="s">
         <v>68</v>
       </c>
       <c r="D34" t="s">
@@ -2054,18 +2342,24 @@
       <c r="K34" t="s">
         <v>49</v>
       </c>
-      <c r="L34" s="4" t="s">
+      <c r="L34" s="2" t="s">
         <v>98</v>
       </c>
-    </row>
-    <row r="35" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M34" s="2" t="s">
+        <v>160</v>
+      </c>
+      <c r="N34" s="2" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="35" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>73</v>
       </c>
       <c r="B35" t="s">
         <v>74</v>
       </c>
-      <c r="C35" s="4" t="s">
+      <c r="C35" s="2" t="s">
         <v>69</v>
       </c>
       <c r="D35" t="s">
@@ -2092,18 +2386,24 @@
       <c r="K35" t="s">
         <v>49</v>
       </c>
-      <c r="L35" s="4" t="s">
+      <c r="L35" s="2" t="s">
         <v>97</v>
       </c>
-    </row>
-    <row r="36" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M35" s="2" t="s">
+        <v>162</v>
+      </c>
+      <c r="N35" s="2" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="36" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>72</v>
       </c>
       <c r="B36" t="s">
         <v>54</v>
       </c>
-      <c r="C36" s="4" t="s">
+      <c r="C36" s="2" t="s">
         <v>70</v>
       </c>
       <c r="D36" t="s">
@@ -2130,18 +2430,24 @@
       <c r="K36" t="s">
         <v>49</v>
       </c>
-      <c r="L36" s="4" t="s">
+      <c r="L36" s="2" t="s">
         <v>99</v>
       </c>
-    </row>
-    <row r="37" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M36" s="2" t="s">
+        <v>163</v>
+      </c>
+      <c r="N36" s="2" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="37" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>73</v>
       </c>
       <c r="B37" t="s">
         <v>74</v>
       </c>
-      <c r="C37" s="4" t="s">
+      <c r="C37" s="2" t="s">
         <v>71</v>
       </c>
       <c r="D37" t="s">
@@ -2168,12 +2474,23 @@
       <c r="K37" t="s">
         <v>49</v>
       </c>
-      <c r="L37" s="4" t="s">
+      <c r="L37" s="2" t="s">
         <v>100</v>
+      </c>
+      <c r="M37" s="2" t="s">
+        <v>166</v>
+      </c>
+      <c r="N37" s="2" t="s">
+        <v>167</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="D1:E1"/>
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="C1:C2"/>
+    <mergeCell ref="N1:N2"/>
+    <mergeCell ref="B1:B2"/>
     <mergeCell ref="M1:M2"/>
     <mergeCell ref="I1:J1"/>
     <mergeCell ref="F1:F2"/>
@@ -2181,11 +2498,6 @@
     <mergeCell ref="H1:H2"/>
     <mergeCell ref="K1:K2"/>
     <mergeCell ref="L1:L2"/>
-    <mergeCell ref="D1:E1"/>
-    <mergeCell ref="A1:A2"/>
-    <mergeCell ref="C1:C2"/>
-    <mergeCell ref="N1:N2"/>
-    <mergeCell ref="B1:B2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>